<commit_message>
rework sys_simulation of bwaise
</commit_message>
<xml_diff>
--- a/dmsan/bwaise/scores/parameters.xlsx
+++ b/dmsan/bwaise/scores/parameters.xlsx
@@ -478,7 +478,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion e cal [kcal/cap/d]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-e cal [kcal/cap/d]')</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -494,7 +494,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion p veg [g/cap/d]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-p veg [g/cap/d]')</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -510,7 +510,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion p anim [g/cap/d]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-p anim [g/cap/d]')</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -526,7 +526,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion N prot [fraction]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-N prot [fraction]')</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -542,7 +542,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion P prot v [fraction]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-P prot v [fraction]')</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -558,7 +558,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion P prot a [fraction]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-P prot a [fraction]')</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -574,7 +574,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion K cal [g K/1000 kcal]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-K cal [g K/1000 kcal]')</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -590,7 +590,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion N exc [fraction of intake]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-N exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -606,7 +606,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion P exc [fraction of intake]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-P exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -622,7 +622,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion K exc [fraction of intake]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-K exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -638,7 +638,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion e exc [fraction of intake]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-e exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -654,7 +654,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion N ur [fraction of total]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-N ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -670,7 +670,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion P ur [fraction of total]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-P ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -686,7 +686,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion K ur [fraction of total]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-K ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -702,7 +702,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion e fec [fraction of total]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-e fec [fraction of total]')</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -718,7 +718,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion N ur NH3 [fraction of total N in urine]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-N ur NH3 [fraction of total N in urine]')</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -734,7 +734,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion N fec NH3 [fraction of total N in feces]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-N fec NH3 [fraction of total N in feces]')</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -750,7 +750,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion ur exc [g/cap/d]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-ur exc [g/cap/d]')</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -766,7 +766,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion fec exc [g/cap/d]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-fec exc [g/cap/d]')</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -782,7 +782,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion ur moi [fraction]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-ur moi [fraction]')</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -798,7 +798,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion fec moi [fraction]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-fec moi [fraction]')</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -814,7 +814,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion mg ur [g Mg/cap/d]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-Mg ur [g Mg/cap/d]')</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -830,7 +830,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion mg fec [g Mg/cap/d]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-Mg fec [g Mg/cap/d]')</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -846,7 +846,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion ca ur [g Ca/cap/d]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-Ca ur [g Ca/cap/d]')</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -862,7 +862,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Excretion ca fec [g Ca/cap/d]')</t>
+          <t>('Excretion-A1', 'A1-Excretion-Ca fec [g Ca/cap/d]')</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -926,7 +926,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine toilet paper [kg/cap/hr]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-toilet paper [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -942,7 +942,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine flushing water [kg/cap/hr]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-flushing water [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -958,7 +958,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine cleansing water [kg/cap/hr]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-cleansing water [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -974,7 +974,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine desiccant V [m3/cap/hr]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-desiccant V [m3/cap/hr]')</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -990,7 +990,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine COD max decay [fraction of oxygen demand removal]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-cod max decay [fraction of oxygen demand removal]')</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine N max decay [fraction of N removal after N leaching]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-n max decay [fraction of N removal after N leaching]')</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
@@ -1022,7 +1022,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine MCF aq [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-mcf aq [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine n2o EF aq [fraction of N emitted as N2O]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-n2o EF aq [fraction of N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine emptying period [yr]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-emptying period [yr]')</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine sludge accum rate [L/cap/yr]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-sludge accum rate [L/cap/yr]')</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine N leaching [fraction of N input]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-n leaching [fraction of N input]')</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
@@ -1198,7 +1198,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine P leaching [fraction of P input]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-p leaching [fraction of P input]')</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
@@ -1214,7 +1214,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine K leaching [fraction of K input]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-k leaching [fraction of K input]')</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Pit latrine N volatilization [fraction of N input]')</t>
+          <t>('Pit latrine-A2', 'A2-Pit latrine-n volatilization [fraction of N input]')</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>('Sedimentation-A5', 'Sedimentation tau [d]')</t>
+          <t>('Sedimentation-A5', 'A5-Sedimentation-tau [d]')</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>('Sedimentation-A5', 'Sedimentation COD max decay [fraction of retained COD]')</t>
+          <t>('Sedimentation-A5', 'A5-Sedimentation-COD max decay [fraction of retained COD]')</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>('Sedimentation-A5', 'Sedimentation MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('Sedimentation-A5', 'A5-Sedimentation-MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>('Sedimentation-A5', 'Sedimentation N max decay [fraction of N removal]')</t>
+          <t>('Sedimentation-A5', 'A5-Sedimentation-N max decay [fraction of N removal]')</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>('Sedimentation-A5', 'Sedimentation n2o EF decay [fraction of degraded N emitted as N2O]')</t>
+          <t>('Sedimentation-A5', 'A5-Sedimentation-N2O EF decay [fraction of degraded N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>('Sedimentation-A5', 'Sedimentation tank L to W [length/width]')</t>
+          <t>('Sedimentation-A5', 'A5-Sedimentation-tank L to W [length/width]')</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>('Sedimentation-A5', 'Sedimentation tank W to H [width/height (average)]')</t>
+          <t>('Sedimentation-A5', 'A5-Sedimentation-tank W to H [width/height (average)]')</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>('Sedimentation-A5', 'Sedimentation concrete thickness [m]')</t>
+          <t>('Sedimentation-A5', 'A5-Sedimentation-concrete thickness [m]')</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>('Sedimentation-A5', 'Sedimentation roof slope [degree]')</t>
+          <t>('Sedimentation-A5', 'A5-Sedimentation-roof slope [degree]')</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
@@ -1630,7 +1630,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>('Sedimentation-A5', 'Sedimentation roof unit mass [kg/m2]')</t>
+          <t>('Sedimentation-A5', 'A5-Sedimentation-roof unit mass [kg/m2]')</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
@@ -1774,7 +1774,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>('Anaerobic lagoon-A6', 'Anaerobic lagoon COD removal [fraction of total COD]')</t>
+          <t>('Anaerobic lagoon-A6', 'A6-Lagoon-COD removal [fraction of total COD]')</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
@@ -1790,7 +1790,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>('Anaerobic lagoon-A6', 'Anaerobic lagoon COD decay [fraction of retained COD]')</t>
+          <t>('Anaerobic lagoon-A6', 'A6-Lagoon-COD decay [fraction of retained COD]')</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>('Anaerobic lagoon-A6', 'Anaerobic lagoon MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('Anaerobic lagoon-A6', 'A6-Lagoon-MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>('Anaerobic lagoon-A6', 'Anaerobic lagoon N max decay [fraction of N removal]')</t>
+          <t>('Anaerobic lagoon-A6', 'A6-Lagoon-N max decay [fraction of N removal]')</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
@@ -1838,7 +1838,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>('Anaerobic lagoon-A6', 'Anaerobic lagoon n2o EF decay [fraction of degraded N emitted as N2O]')</t>
+          <t>('Anaerobic lagoon-A6', 'A6-Lagoon-N2O EF decay [fraction of degraded N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
@@ -1854,7 +1854,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>('Anaerobic lagoon-A6', 'Anaerobic lagoon liner unit mass [kg/m2]')</t>
+          <t>('Anaerobic lagoon-A6', 'A6-Lagoon-liner unit mass [kg/m2]')</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
@@ -1886,7 +1886,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-A7', 'Facultative lagoon COD removal [fraction of total COD]')</t>
+          <t>('Facultative lagoon-A7', 'A7-Lagoon-COD removal [fraction of total COD]')</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
@@ -1902,7 +1902,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-A7', 'Facultative lagoon COD decay [fraction of retained COD]')</t>
+          <t>('Facultative lagoon-A7', 'A7-Lagoon-COD decay [fraction of retained COD]')</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-A7', 'Facultative lagoon MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('Facultative lagoon-A7', 'A7-Lagoon-MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C92" t="inlineStr"/>
@@ -1934,7 +1934,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-A7', 'Facultative lagoon N max decay [fraction of N removal]')</t>
+          <t>('Facultative lagoon-A7', 'A7-Lagoon-N max decay [fraction of N removal]')</t>
         </is>
       </c>
       <c r="C93" t="inlineStr"/>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-A7', 'Facultative lagoon n2o EF decay [fraction of of degraded N emitted as N2O]')</t>
+          <t>('Facultative lagoon-A7', 'A7-Lagoon-N2O EF decay [fraction of of degraded N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C94" t="inlineStr"/>
@@ -1966,7 +1966,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-A7', 'Facultative lagoon P removal [fraction of P removal]')</t>
+          <t>('Facultative lagoon-A7', 'A7-Lagoon-P removal [fraction of P removal]')</t>
         </is>
       </c>
       <c r="C95" t="inlineStr"/>
@@ -1982,7 +1982,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-A7', 'Facultative lagoon liner unit mass [kg/m2]')</t>
+          <t>('Facultative lagoon-A7', 'A7-Lagoon-liner unit mass [kg/m2]')</t>
         </is>
       </c>
       <c r="C96" t="inlineStr"/>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-A8', 'Drying bed tau [d]')</t>
+          <t>('Unplanted drying bed-A8', 'A8-Drying bed-tau [d]')</t>
         </is>
       </c>
       <c r="C98" t="inlineStr"/>
@@ -2030,7 +2030,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-A8', 'Drying bed COD max decay [fraction of total COD]')</t>
+          <t>('Unplanted drying bed-A8', 'A8-Drying bed-cod max decay [fraction of total COD]')</t>
         </is>
       </c>
       <c r="C99" t="inlineStr"/>
@@ -2046,7 +2046,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-A8', 'Drying bed MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('Unplanted drying bed-A8', 'A8-Drying bed-mcf decay [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C100" t="inlineStr"/>
@@ -2062,7 +2062,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-A8', 'Drying bed N max decay [fraction of N removal]')</t>
+          <t>('Unplanted drying bed-A8', 'A8-Drying bed-n max decay [fraction of N removal]')</t>
         </is>
       </c>
       <c r="C101" t="inlineStr"/>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-A8', 'Drying bed n2o EF decay [fraction of degraded N emitted as N2O]')</t>
+          <t>('Unplanted drying bed-A8', 'A8-Drying bed-n2o EF decay [fraction of degraded N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C102" t="inlineStr"/>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-A8', 'Drying bed column H [m]')</t>
+          <t>('Unplanted drying bed-A8', 'A8-Drying bed-column H [m]')</t>
         </is>
       </c>
       <c r="C103" t="inlineStr"/>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-A8', 'Drying bed column unit mass [kg/m]')</t>
+          <t>('Unplanted drying bed-A8', 'A8-Drying bed-column unit mass [kg/m]')</t>
         </is>
       </c>
       <c r="C104" t="inlineStr"/>
@@ -2126,7 +2126,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-A8', 'Drying bed concrete thickness [m]')</t>
+          <t>('Unplanted drying bed-A8', 'A8-Drying bed-concrete thickness [m]')</t>
         </is>
       </c>
       <c r="C105" t="inlineStr"/>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-A8', 'Drying bed cover slope [degree]')</t>
+          <t>('Unplanted drying bed-A8', 'A8-Drying bed-cover slope [degree]')</t>
         </is>
       </c>
       <c r="C106" t="inlineStr"/>
@@ -2158,7 +2158,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-A8', 'Drying bed cover unit mass [kg/m2]')</t>
+          <t>('Unplanted drying bed-A8', 'A8-Drying bed-cover unit mass [kg/m2]')</t>
         </is>
       </c>
       <c r="C107" t="inlineStr"/>
@@ -2254,7 +2254,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>('TEA/LCA', 'Plant lifetime [yr]')</t>
+          <t>('LCA', 'Brick H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C113" t="inlineStr"/>
@@ -2270,7 +2270,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Brick H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C114" t="inlineStr"/>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Brick H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C115" t="inlineStr"/>
@@ -2302,7 +2302,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Cement H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C116" t="inlineStr"/>
@@ -2318,7 +2318,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Cement H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C117" t="inlineStr"/>
@@ -2334,7 +2334,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Cement H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C118" t="inlineStr"/>
@@ -2350,7 +2350,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Concrete H resources total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C119" t="inlineStr"/>
@@ -2366,7 +2366,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete H ecosystem quality total CF [points/m3]')</t>
+          <t>('LCA', 'Concrete H ecosystem quality total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C120" t="inlineStr"/>
@@ -2382,7 +2382,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete H human health total CF [points/m3]')</t>
+          <t>('LCA', 'Concrete H human health total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C121" t="inlineStr"/>
@@ -2398,7 +2398,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete H resources total CF [points/m3]')</t>
+          <t>('LCA', 'Excavation H resources total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C122" t="inlineStr"/>
@@ -2414,7 +2414,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation H ecosystem quality total CF [points/m3]')</t>
+          <t>('LCA', 'Excavation H ecosystem quality total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C123" t="inlineStr"/>
@@ -2430,7 +2430,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation H human health total CF [points/m3]')</t>
+          <t>('LCA', 'Excavation H human health total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C124" t="inlineStr"/>
@@ -2446,7 +2446,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation H resources total CF [points/m3]')</t>
+          <t>('LCA', 'Gravel H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C125" t="inlineStr"/>
@@ -2462,7 +2462,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Gravel H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C126" t="inlineStr"/>
@@ -2478,7 +2478,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Gravel H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C127" t="inlineStr"/>
@@ -2494,7 +2494,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Plastic H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C128" t="inlineStr"/>
@@ -2510,7 +2510,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Plastic H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C129" t="inlineStr"/>
@@ -2526,7 +2526,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Plastic H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C130" t="inlineStr"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Sand H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C131" t="inlineStr"/>
@@ -2558,7 +2558,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Sand H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C132" t="inlineStr"/>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Sand H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C133" t="inlineStr"/>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C134" t="inlineStr"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C135" t="inlineStr"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C136" t="inlineStr"/>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C137" t="inlineStr"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C138" t="inlineStr"/>
@@ -2670,7 +2670,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C139" t="inlineStr"/>
@@ -2686,7 +2686,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Steel H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C140" t="inlineStr"/>
@@ -2702,7 +2702,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Steel H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C141" t="inlineStr"/>
@@ -2718,7 +2718,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Steel H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C142" t="inlineStr"/>
@@ -2734,7 +2734,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Wood H resources total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C143" t="inlineStr"/>
@@ -2750,7 +2750,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood H ecosystem quality total CF [points/m3]')</t>
+          <t>('LCA', 'Wood H ecosystem quality total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C144" t="inlineStr"/>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood H human health total CF [points/m3]')</t>
+          <t>('LCA', 'Wood H human health total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C145" t="inlineStr"/>
@@ -2782,7 +2782,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood H resources total CF [points/m3]')</t>
+          <t>('LCA', 'Trucking H resources total CF [points/ton kilometer]')</t>
         </is>
       </c>
       <c r="C146" t="inlineStr"/>
@@ -2798,7 +2798,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking H ecosystem quality total CF [points/tonne*km]')</t>
+          <t>('LCA', 'Trucking H ecosystem quality total CF [points/ton kilometer]')</t>
         </is>
       </c>
       <c r="C147" t="inlineStr"/>
@@ -2814,7 +2814,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking H human health total CF [points/tonne*km]')</t>
+          <t>('LCA', 'Trucking H human health total CF [points/ton kilometer]')</t>
         </is>
       </c>
       <c r="C148" t="inlineStr"/>
@@ -2830,7 +2830,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking H resources total CF [points/tonne*km]')</t>
+          <t>('LCA', 'N item H resources total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C149" t="inlineStr"/>
@@ -2878,7 +2878,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>('LCA', 'N item H resources total CF [points/kg]')</t>
+          <t>('LCA', 'P item H resources total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C152" t="inlineStr"/>
@@ -2926,7 +2926,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>('LCA', 'P item H resources total CF [points/kg]')</t>
+          <t>('LCA', 'K item H resources total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C155" t="inlineStr"/>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>('LCA', 'K item H resources total CF [points/kg]')</t>
+          <t>('LCA', 'E item H resources total CF [points/kilowatt hour]')</t>
         </is>
       </c>
       <c r="C158" t="inlineStr"/>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>('LCA', 'E item H ecosystem quality total CF [points/kWh]')</t>
+          <t>('LCA', 'E item H ecosystem quality total CF [points/kilowatt hour]')</t>
         </is>
       </c>
       <c r="C159" t="inlineStr"/>
@@ -3006,7 +3006,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>('LCA', 'E item H human health total CF [points/kWh]')</t>
+          <t>('LCA', 'E item H human health total CF [points/kilowatt hour]')</t>
         </is>
       </c>
       <c r="C160" t="inlineStr"/>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>('LCA', 'E item H resources total CF [points/kWh]')</t>
+          <t>('TEA/LCA', 'Plant lifetime [yr]')</t>
         </is>
       </c>
       <c r="C161" t="inlineStr"/>
@@ -3222,7 +3222,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion e cal [kcal/cap/d]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-e cal [kcal/cap/d]')</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -3238,7 +3238,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion p veg [g/cap/d]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-p veg [g/cap/d]')</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion p anim [g/cap/d]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-p anim [g/cap/d]')</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -3270,7 +3270,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion N prot [fraction]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-N prot [fraction]')</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion P prot v [fraction]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-P prot v [fraction]')</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -3302,7 +3302,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion P prot a [fraction]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-P prot a [fraction]')</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion K cal [g K/1000 kcal]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-K cal [g K/1000 kcal]')</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -3334,7 +3334,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion N exc [fraction of intake]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-N exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -3350,7 +3350,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion P exc [fraction of intake]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-P exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -3366,7 +3366,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion K exc [fraction of intake]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-K exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -3382,7 +3382,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion e exc [fraction of intake]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-e exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -3398,7 +3398,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion N ur [fraction of total]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-N ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -3414,7 +3414,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion P ur [fraction of total]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-P ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -3430,7 +3430,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion K ur [fraction of total]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-K ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion e fec [fraction of total]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-e fec [fraction of total]')</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -3462,7 +3462,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion N ur NH3 [fraction of total N in urine]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-N ur NH3 [fraction of total N in urine]')</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion N fec NH3 [fraction of total N in feces]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-N fec NH3 [fraction of total N in feces]')</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion ur exc [g/cap/d]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-ur exc [g/cap/d]')</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion fec exc [g/cap/d]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-fec exc [g/cap/d]')</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion ur moi [fraction]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-ur moi [fraction]')</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -3542,7 +3542,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion fec moi [fraction]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-fec moi [fraction]')</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -3558,7 +3558,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion mg ur [g Mg/cap/d]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-Mg ur [g Mg/cap/d]')</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -3574,7 +3574,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion mg fec [g Mg/cap/d]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-Mg fec [g Mg/cap/d]')</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -3590,7 +3590,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion ca ur [g Ca/cap/d]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-Ca ur [g Ca/cap/d]')</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -3606,7 +3606,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Excretion ca fec [g Ca/cap/d]')</t>
+          <t>('Excretion-B1', 'B1-Excretion-Ca fec [g Ca/cap/d]')</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -3670,7 +3670,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine toilet paper [kg/cap/hr]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-toilet paper [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -3686,7 +3686,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine flushing water [kg/cap/hr]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-flushing water [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -3702,7 +3702,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine cleansing water [kg/cap/hr]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-cleansing water [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -3718,7 +3718,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine desiccant V [m3/cap/hr]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-desiccant V [m3/cap/hr]')</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -3734,7 +3734,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine COD max decay [fraction of oxygen demand removal]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-cod max decay [fraction of oxygen demand removal]')</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
@@ -3750,7 +3750,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine N max decay [fraction of N removal after N leaching]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-n max decay [fraction of N removal after N leaching]')</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine MCF aq [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-mcf aq [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
@@ -3782,7 +3782,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine n2o EF aq [fraction of N emitted as N2O]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-n2o EF aq [fraction of N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
@@ -3894,7 +3894,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine emptying period [yr]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-emptying period [yr]')</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -3910,7 +3910,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine sludge accum rate [L/cap/yr]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-sludge accum rate [L/cap/yr]')</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine N leaching [fraction of N input]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-n leaching [fraction of N input]')</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
@@ -3942,7 +3942,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine P leaching [fraction of P input]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-p leaching [fraction of P input]')</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
@@ -3958,7 +3958,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine K leaching [fraction of K input]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-k leaching [fraction of K input]')</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
@@ -3974,7 +3974,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>('Pit latrine-B2', 'Pit latrine N volatilization [fraction of N input]')</t>
+          <t>('Pit latrine-B2', 'B2-Pit latrine-n volatilization [fraction of N input]')</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>('Anaerobic baffled reactor-B5', 'Anaerobic baffled reactor tau [d]')</t>
+          <t>('Anaerobic baffled reactor-B5', 'B5-Anaerobic baffled reactor-tau [d]')</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>('Anaerobic baffled reactor-B5', 'Anaerobic baffled reactor COD removal [fraction of total COD]')</t>
+          <t>('Anaerobic baffled reactor-B5', 'B5-Anaerobic baffled reactor-cod removal [fraction of total COD]')</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
@@ -4262,7 +4262,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>('Anaerobic baffled reactor-B5', 'Anaerobic baffled reactor N removal [fraction of N removed]')</t>
+          <t>('Anaerobic baffled reactor-B5', 'B5-Anaerobic baffled reactor-n removal [fraction of N removed]')</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
@@ -4278,7 +4278,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>('Anaerobic baffled reactor-B5', 'Anaerobic baffled reactor N max decay [fraction of N removal]')</t>
+          <t>('Anaerobic baffled reactor-B5', 'B5-Anaerobic baffled reactor-n max decay [fraction of N removal]')</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
@@ -4294,7 +4294,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>('Anaerobic baffled reactor-B5', 'Anaerobic baffled reactor n2o EF decay [fraction of degraded N emitted as N2O]')</t>
+          <t>('Anaerobic baffled reactor-B5', 'B5-Anaerobic baffled reactor-n2o EF decay [fraction of degraded N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
@@ -4310,7 +4310,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>('Anaerobic baffled reactor-B5', 'Anaerobic baffled reactor reactor H [m]')</t>
+          <t>('Anaerobic baffled reactor-B5', 'B5-Anaerobic baffled reactor-reactor H [m]')</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>('Anaerobic baffled reactor-B5', 'Anaerobic baffled reactor add concrete [fraction of total]')</t>
+          <t>('Anaerobic baffled reactor-B5', 'B5-Anaerobic baffled reactor-add concrete [fraction of total]')</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
@@ -4342,7 +4342,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>('Anaerobic baffled reactor-B5', 'Anaerobic baffled reactor concrete thickness [m]')</t>
+          <t>('Anaerobic baffled reactor-B5', 'B5-Anaerobic baffled reactor-concrete thickness [m]')</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
@@ -4502,7 +4502,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'Liquid treatment bed tau [d]')</t>
+          <t>('Liquid treatment bed-B7', 'B7-Liquid treatment bed-tau [d]')</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
@@ -4518,7 +4518,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'Liquid treatment bed COD max decay [% of total COD]')</t>
+          <t>('Liquid treatment bed-B7', 'B7-Liquid treatment bed-cod max decay [% of total COD]')</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
@@ -4534,7 +4534,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'Liquid treatment bed MCF decay [% anaerobic conversion of degraded COD]')</t>
+          <t>('Liquid treatment bed-B7', 'B7-Liquid treatment bed-mcf decay [% anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
@@ -4550,7 +4550,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'Liquid treatment bed N max decay [% N removal]')</t>
+          <t>('Liquid treatment bed-B7', 'B7-Liquid treatment bed-n max decay [% N removal]')</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'Liquid treatment bed n2o EF decay [% of degraded N emitted as N2O]')</t>
+          <t>('Liquid treatment bed-B7', 'B7-Liquid treatment bed-n2o EF decay [% of degraded N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'Liquid treatment bed bed H [m]')</t>
+          <t>('Liquid treatment bed-B7', 'B7-Liquid treatment bed-bed H [m]')</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
@@ -4598,7 +4598,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'Liquid treatment bed concrete thickness [m]')</t>
+          <t>('Liquid treatment bed-B7', 'B7-Liquid treatment bed-concrete thickness [m]')</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
@@ -4614,7 +4614,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>('Planted drying bed-B8', 'Drying bed tau [d]')</t>
+          <t>('Planted drying bed-B8', 'B8-Drying bed-tau [d]')</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
@@ -4630,7 +4630,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>('Planted drying bed-B8', 'Drying bed COD max decay [fraction of total COD]')</t>
+          <t>('Planted drying bed-B8', 'B8-Drying bed-cod max decay [fraction of total COD]')</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
@@ -4646,7 +4646,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>('Planted drying bed-B8', 'Drying bed MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('Planted drying bed-B8', 'B8-Drying bed-mcf decay [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C92" t="inlineStr"/>
@@ -4662,7 +4662,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>('Planted drying bed-B8', 'Drying bed N max decay [fraction of N removal]')</t>
+          <t>('Planted drying bed-B8', 'B8-Drying bed-n max decay [fraction of N removal]')</t>
         </is>
       </c>
       <c r="C93" t="inlineStr"/>
@@ -4678,7 +4678,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>('Planted drying bed-B8', 'Drying bed n2o EF decay [fraction of degraded N emitted as N2O]')</t>
+          <t>('Planted drying bed-B8', 'B8-Drying bed-n2o EF decay [fraction of degraded N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C94" t="inlineStr"/>
@@ -4694,7 +4694,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>('Planted drying bed-B8', 'Drying bed column H [m]')</t>
+          <t>('Planted drying bed-B8', 'B8-Drying bed-column H [m]')</t>
         </is>
       </c>
       <c r="C95" t="inlineStr"/>
@@ -4710,7 +4710,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>('Planted drying bed-B8', 'Drying bed column unit mass [kg/m]')</t>
+          <t>('Planted drying bed-B8', 'B8-Drying bed-column unit mass [kg/m]')</t>
         </is>
       </c>
       <c r="C96" t="inlineStr"/>
@@ -4726,7 +4726,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>('Planted drying bed-B8', 'Drying bed concrete thickness [m]')</t>
+          <t>('Planted drying bed-B8', 'B8-Drying bed-concrete thickness [m]')</t>
         </is>
       </c>
       <c r="C97" t="inlineStr"/>
@@ -4742,7 +4742,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>('Planted drying bed-B8', 'Drying bed cover slope [degree]')</t>
+          <t>('Planted drying bed-B8', 'B8-Drying bed-cover slope [degree]')</t>
         </is>
       </c>
       <c r="C98" t="inlineStr"/>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>('Planted drying bed-B8', 'Drying bed cover unit mass [kg/m2]')</t>
+          <t>('Planted drying bed-B8', 'B8-Drying bed-cover unit mass [kg/m2]')</t>
         </is>
       </c>
       <c r="C99" t="inlineStr"/>
@@ -4854,7 +4854,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>('TEA/LCA', 'Plant lifetime [yr]')</t>
+          <t>('LCA', 'Brick H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C105" t="inlineStr"/>
@@ -4870,7 +4870,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>('TEA/LCA', 'Liquid petroleum gas energy [MJ/kg]')</t>
+          <t>('LCA', 'Brick H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C106" t="inlineStr"/>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Brick H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C107" t="inlineStr"/>
@@ -4902,7 +4902,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Cement H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C108" t="inlineStr"/>
@@ -4918,7 +4918,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Cement H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C109" t="inlineStr"/>
@@ -4934,7 +4934,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Cement H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C110" t="inlineStr"/>
@@ -4950,7 +4950,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Concrete H resources total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C111" t="inlineStr"/>
@@ -4966,7 +4966,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Concrete H ecosystem quality total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C112" t="inlineStr"/>
@@ -4982,7 +4982,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete H ecosystem quality total CF [points/m3]')</t>
+          <t>('LCA', 'Concrete H human health total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C113" t="inlineStr"/>
@@ -4998,7 +4998,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete H human health total CF [points/m3]')</t>
+          <t>('LCA', 'Excavation H resources total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C114" t="inlineStr"/>
@@ -5014,7 +5014,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete H resources total CF [points/m3]')</t>
+          <t>('LCA', 'Excavation H ecosystem quality total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C115" t="inlineStr"/>
@@ -5030,7 +5030,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation H ecosystem quality total CF [points/m3]')</t>
+          <t>('LCA', 'Excavation H human health total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C116" t="inlineStr"/>
@@ -5046,7 +5046,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation H human health total CF [points/m3]')</t>
+          <t>('LCA', 'Gravel H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C117" t="inlineStr"/>
@@ -5062,7 +5062,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation H resources total CF [points/m3]')</t>
+          <t>('LCA', 'Gravel H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C118" t="inlineStr"/>
@@ -5078,7 +5078,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Gravel H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C119" t="inlineStr"/>
@@ -5094,7 +5094,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Plastic H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C120" t="inlineStr"/>
@@ -5110,7 +5110,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Plastic H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C121" t="inlineStr"/>
@@ -5126,7 +5126,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Plastic H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C122" t="inlineStr"/>
@@ -5142,7 +5142,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Sand H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C123" t="inlineStr"/>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Sand H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C124" t="inlineStr"/>
@@ -5174,7 +5174,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Sand H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C125" t="inlineStr"/>
@@ -5190,7 +5190,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C126" t="inlineStr"/>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C127" t="inlineStr"/>
@@ -5222,7 +5222,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C128" t="inlineStr"/>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C129" t="inlineStr"/>
@@ -5254,7 +5254,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C130" t="inlineStr"/>
@@ -5270,7 +5270,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C131" t="inlineStr"/>
@@ -5286,7 +5286,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Steel H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C132" t="inlineStr"/>
@@ -5302,7 +5302,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Steel H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C133" t="inlineStr"/>
@@ -5318,7 +5318,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Steel H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C134" t="inlineStr"/>
@@ -5334,7 +5334,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Wood H resources total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C135" t="inlineStr"/>
@@ -5350,7 +5350,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Wood H ecosystem quality total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C136" t="inlineStr"/>
@@ -5366,7 +5366,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood H ecosystem quality total CF [points/m3]')</t>
+          <t>('LCA', 'Wood H human health total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C137" t="inlineStr"/>
@@ -5382,7 +5382,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood H human health total CF [points/m3]')</t>
+          <t>('LCA', 'Trucking H resources total CF [points/ton kilometer]')</t>
         </is>
       </c>
       <c r="C138" t="inlineStr"/>
@@ -5398,7 +5398,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood H resources total CF [points/m3]')</t>
+          <t>('LCA', 'Trucking H ecosystem quality total CF [points/ton kilometer]')</t>
         </is>
       </c>
       <c r="C139" t="inlineStr"/>
@@ -5414,7 +5414,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking H ecosystem quality total CF [points/tonne*km]')</t>
+          <t>('LCA', 'Trucking H human health total CF [points/ton kilometer]')</t>
         </is>
       </c>
       <c r="C140" t="inlineStr"/>
@@ -5430,7 +5430,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking H human health total CF [points/tonne*km]')</t>
+          <t>('LCA', 'Biogas item H resources total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C141" t="inlineStr"/>
@@ -5446,7 +5446,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking H resources total CF [points/tonne*km]')</t>
+          <t>('LCA', 'Biogas item H ecosystem quality total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C142" t="inlineStr"/>
@@ -5462,7 +5462,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>('LCA', 'Biogas item H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Biogas item H human health total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C143" t="inlineStr"/>
@@ -5478,7 +5478,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>('LCA', 'Biogas item H human health total CF [points/kg]')</t>
+          <t>('LCA', 'N item H resources total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C144" t="inlineStr"/>
@@ -5494,7 +5494,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>('LCA', 'Biogas item H resources total CF [points/kg]')</t>
+          <t>('LCA', 'N item H ecosystem quality total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C145" t="inlineStr"/>
@@ -5510,7 +5510,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>('LCA', 'N item H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'N item H human health total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C146" t="inlineStr"/>
@@ -5526,7 +5526,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>('LCA', 'N item H human health total CF [points/kg]')</t>
+          <t>('LCA', 'P item H resources total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C147" t="inlineStr"/>
@@ -5542,7 +5542,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>('LCA', 'N item H resources total CF [points/kg]')</t>
+          <t>('LCA', 'P item H ecosystem quality total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C148" t="inlineStr"/>
@@ -5558,7 +5558,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>('LCA', 'P item H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'P item H human health total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C149" t="inlineStr"/>
@@ -5574,7 +5574,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>('LCA', 'P item H human health total CF [points/kg]')</t>
+          <t>('LCA', 'K item H resources total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C150" t="inlineStr"/>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>('LCA', 'P item H resources total CF [points/kg]')</t>
+          <t>('LCA', 'K item H ecosystem quality total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C151" t="inlineStr"/>
@@ -5606,7 +5606,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>('LCA', 'K item H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'K item H human health total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C152" t="inlineStr"/>
@@ -5622,7 +5622,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>('LCA', 'K item H human health total CF [points/kg]')</t>
+          <t>('LCA', 'E item H resources total CF [points/kilowatt hour]')</t>
         </is>
       </c>
       <c r="C153" t="inlineStr"/>
@@ -5638,7 +5638,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>('LCA', 'K item H resources total CF [points/kg]')</t>
+          <t>('LCA', 'E item H ecosystem quality total CF [points/kilowatt hour]')</t>
         </is>
       </c>
       <c r="C154" t="inlineStr"/>
@@ -5654,7 +5654,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>('LCA', 'E item H ecosystem quality total CF [points/kWh]')</t>
+          <t>('LCA', 'E item H human health total CF [points/kilowatt hour]')</t>
         </is>
       </c>
       <c r="C155" t="inlineStr"/>
@@ -5670,7 +5670,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>('LCA', 'E item H human health total CF [points/kWh]')</t>
+          <t>('TEA/LCA', 'Plant lifetime [yr]')</t>
         </is>
       </c>
       <c r="C156" t="inlineStr"/>
@@ -5686,7 +5686,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>('LCA', 'E item H resources total CF [points/kWh]')</t>
+          <t>('TEA/LCA', 'Liquid petroleum gas energy [MJ/kg]')</t>
         </is>
       </c>
       <c r="C157" t="inlineStr"/>
@@ -5902,7 +5902,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion e cal [kcal/cap/d]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-e cal [kcal/cap/d]')</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -5918,7 +5918,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion p veg [g/cap/d]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-p veg [g/cap/d]')</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -5934,7 +5934,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion p anim [g/cap/d]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-p anim [g/cap/d]')</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -5950,7 +5950,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion N prot [fraction]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-N prot [fraction]')</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -5966,7 +5966,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion P prot v [fraction]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-P prot v [fraction]')</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -5982,7 +5982,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion P prot a [fraction]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-P prot a [fraction]')</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -5998,7 +5998,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion K cal [g K/1000 kcal]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-K cal [g K/1000 kcal]')</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -6014,7 +6014,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion N exc [fraction of intake]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-N exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -6030,7 +6030,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion P exc [fraction of intake]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-P exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -6046,7 +6046,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion K exc [fraction of intake]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-K exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -6062,7 +6062,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion e exc [fraction of intake]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-e exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -6078,7 +6078,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion N ur [fraction of total]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-N ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -6094,7 +6094,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion P ur [fraction of total]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-P ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -6110,7 +6110,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion K ur [fraction of total]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-K ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -6126,7 +6126,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion e fec [fraction of total]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-e fec [fraction of total]')</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -6142,7 +6142,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion N ur NH3 [fraction of total N in urine]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-N ur NH3 [fraction of total N in urine]')</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion N fec NH3 [fraction of total N in feces]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-N fec NH3 [fraction of total N in feces]')</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -6174,7 +6174,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion ur exc [g/cap/d]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-ur exc [g/cap/d]')</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -6190,7 +6190,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion fec exc [g/cap/d]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-fec exc [g/cap/d]')</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion ur moi [fraction]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-ur moi [fraction]')</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -6222,7 +6222,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion fec moi [fraction]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-fec moi [fraction]')</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -6238,7 +6238,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion mg ur [g Mg/cap/d]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-Mg ur [g Mg/cap/d]')</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -6254,7 +6254,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion mg fec [g Mg/cap/d]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-Mg fec [g Mg/cap/d]')</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion ca ur [g Ca/cap/d]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-Ca ur [g Ca/cap/d]')</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -6286,7 +6286,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>('Excretion-C1', 'Excretion ca fec [g Ca/cap/d]')</t>
+          <t>('Excretion-C1', 'C1-Excretion-Ca fec [g Ca/cap/d]')</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -6350,7 +6350,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT toilet paper [kg/cap/hr]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-toilet paper [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -6366,7 +6366,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT flushing water [kg/cap/hr]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-flushing water [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -6382,7 +6382,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT cleansing water [kg/cap/hr]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-cleansing water [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -6398,7 +6398,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT desiccant V [m3/cap/hr]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-desiccant V [m3/cap/hr]')</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -6414,7 +6414,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT COD max decay [fraction of oxygen demand removal]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-COD max decay [fraction of oxygen demand removal]')</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -6430,7 +6430,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT N max decay [fraction of N removal after N leaching]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-N max decay [fraction of N removal after N leaching]')</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
@@ -6446,7 +6446,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT MCF aq [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-MCF aq [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
@@ -6462,7 +6462,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT n2o EF aq [fraction of N emitted as N2O]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-N2O EF aq [fraction of N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
@@ -6574,7 +6574,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT collection period [d]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-collection period [d]')</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -6590,7 +6590,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT N volatilization [fraction of total N]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-N volatilization [fraction of total N]')</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -6606,7 +6606,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT struvite p ksp [-]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-struvite p ksp [-]')</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
@@ -6622,7 +6622,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT prep sludge [fraction of total precipitate appearing as sludge that settles and can be removed]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-prep sludge [fraction of total precipitate appearing as sludge that settles and can be removed]')</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
@@ -6638,7 +6638,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT log removal [log unit]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-log removal [log unit]')</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
@@ -6654,7 +6654,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT ur p H [pH unit]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-ur p H [pH unit]')</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
@@ -6670,7 +6670,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
@@ -6686,7 +6686,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT n2o EF decay [fraction of N emitted as N2O]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-N2O EF decay [fraction of N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
@@ -6702,7 +6702,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT fec moi min [fraction]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-fec moi min [fraction]')</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
@@ -6718,7 +6718,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>('UDDT-C2', 'UDDT fec moi red rate [1/d]')</t>
+          <t>('UDDT-C2', 'C2-UDDT-fec moi red rate [1/d]')</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
@@ -6958,7 +6958,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>('Anaerobic lagoon-C6', 'Anaerobic lagoon COD removal [fraction of total COD]')</t>
+          <t>('Anaerobic lagoon-C6', 'C6-Lagoon-COD removal [fraction of total COD]')</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
@@ -6974,7 +6974,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>('Anaerobic lagoon-C6', 'Anaerobic lagoon COD decay [fraction of retained COD]')</t>
+          <t>('Anaerobic lagoon-C6', 'C6-Lagoon-COD decay [fraction of retained COD]')</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
@@ -6990,7 +6990,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>('Anaerobic lagoon-C6', 'Anaerobic lagoon MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('Anaerobic lagoon-C6', 'C6-Lagoon-MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
@@ -7006,7 +7006,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>('Anaerobic lagoon-C6', 'Anaerobic lagoon N max decay [fraction of N removal]')</t>
+          <t>('Anaerobic lagoon-C6', 'C6-Lagoon-N max decay [fraction of N removal]')</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
@@ -7022,7 +7022,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>('Anaerobic lagoon-C6', 'Anaerobic lagoon n2o EF decay [fraction of degraded N emitted as N2O]')</t>
+          <t>('Anaerobic lagoon-C6', 'C6-Lagoon-N2O EF decay [fraction of degraded N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
@@ -7038,7 +7038,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>('Anaerobic lagoon-C6', 'Anaerobic lagoon liner unit mass [kg/m2]')</t>
+          <t>('Anaerobic lagoon-C6', 'C6-Lagoon-liner unit mass [kg/m2]')</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
@@ -7070,7 +7070,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-C7', 'Facultative lagoon COD removal [fraction of total COD]')</t>
+          <t>('Facultative lagoon-C7', 'C7-Lagoon-COD removal [fraction of total COD]')</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
@@ -7086,7 +7086,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-C7', 'Facultative lagoon COD decay [fraction of retained COD]')</t>
+          <t>('Facultative lagoon-C7', 'C7-Lagoon-COD decay [fraction of retained COD]')</t>
         </is>
       </c>
       <c r="C76" t="inlineStr"/>
@@ -7102,7 +7102,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-C7', 'Facultative lagoon MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('Facultative lagoon-C7', 'C7-Lagoon-MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
@@ -7118,7 +7118,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-C7', 'Facultative lagoon N max decay [fraction of N removal]')</t>
+          <t>('Facultative lagoon-C7', 'C7-Lagoon-N max decay [fraction of N removal]')</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
@@ -7134,7 +7134,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-C7', 'Facultative lagoon n2o EF decay [fraction of of degraded N emitted as N2O]')</t>
+          <t>('Facultative lagoon-C7', 'C7-Lagoon-N2O EF decay [fraction of of degraded N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
@@ -7150,7 +7150,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-C7', 'Facultative lagoon P removal [fraction of P removal]')</t>
+          <t>('Facultative lagoon-C7', 'C7-Lagoon-P removal [fraction of P removal]')</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
@@ -7166,7 +7166,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>('Facultative lagoon-C7', 'Facultative lagoon liner unit mass [kg/m2]')</t>
+          <t>('Facultative lagoon-C7', 'C7-Lagoon-liner unit mass [kg/m2]')</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
@@ -7198,7 +7198,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-C8', 'Drying bed tau [d]')</t>
+          <t>('Unplanted drying bed-C8', 'C8-Drying bed-tau [d]')</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
@@ -7214,7 +7214,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-C8', 'Drying bed COD max decay [fraction of total COD]')</t>
+          <t>('Unplanted drying bed-C8', 'C8-Drying bed-cod max decay [fraction of total COD]')</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
@@ -7230,7 +7230,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-C8', 'Drying bed MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('Unplanted drying bed-C8', 'C8-Drying bed-mcf decay [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
@@ -7246,7 +7246,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-C8', 'Drying bed N max decay [fraction of N removal]')</t>
+          <t>('Unplanted drying bed-C8', 'C8-Drying bed-n max decay [fraction of N removal]')</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
@@ -7262,7 +7262,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-C8', 'Drying bed n2o EF decay [fraction of degraded N emitted as N2O]')</t>
+          <t>('Unplanted drying bed-C8', 'C8-Drying bed-n2o EF decay [fraction of degraded N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
@@ -7278,7 +7278,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-C8', 'Drying bed column H [m]')</t>
+          <t>('Unplanted drying bed-C8', 'C8-Drying bed-column H [m]')</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
@@ -7294,7 +7294,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-C8', 'Drying bed column unit mass [kg/m]')</t>
+          <t>('Unplanted drying bed-C8', 'C8-Drying bed-column unit mass [kg/m]')</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
@@ -7310,7 +7310,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-C8', 'Drying bed concrete thickness [m]')</t>
+          <t>('Unplanted drying bed-C8', 'C8-Drying bed-concrete thickness [m]')</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
@@ -7326,7 +7326,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-C8', 'Drying bed cover slope [degree]')</t>
+          <t>('Unplanted drying bed-C8', 'C8-Drying bed-cover slope [degree]')</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
@@ -7342,7 +7342,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>('Unplanted drying bed-C8', 'Drying bed cover unit mass [kg/m2]')</t>
+          <t>('Unplanted drying bed-C8', 'C8-Drying bed-cover unit mass [kg/m2]')</t>
         </is>
       </c>
       <c r="C92" t="inlineStr"/>
@@ -7438,7 +7438,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>('TEA/LCA', 'Plant lifetime [yr]')</t>
+          <t>('LCA', 'Brick H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C98" t="inlineStr"/>
@@ -7454,7 +7454,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Brick H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C99" t="inlineStr"/>
@@ -7470,7 +7470,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Brick H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C100" t="inlineStr"/>
@@ -7486,7 +7486,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>('LCA', 'Brick H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Cement H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C101" t="inlineStr"/>
@@ -7502,7 +7502,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Cement H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C102" t="inlineStr"/>
@@ -7518,7 +7518,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Cement H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C103" t="inlineStr"/>
@@ -7534,7 +7534,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>('LCA', 'Cement H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Concrete H resources total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C104" t="inlineStr"/>
@@ -7550,7 +7550,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete H ecosystem quality total CF [points/m3]')</t>
+          <t>('LCA', 'Concrete H ecosystem quality total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C105" t="inlineStr"/>
@@ -7566,7 +7566,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete H human health total CF [points/m3]')</t>
+          <t>('LCA', 'Concrete H human health total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C106" t="inlineStr"/>
@@ -7582,7 +7582,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>('LCA', 'Concrete H resources total CF [points/m3]')</t>
+          <t>('LCA', 'Excavation H resources total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C107" t="inlineStr"/>
@@ -7598,7 +7598,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation H ecosystem quality total CF [points/m3]')</t>
+          <t>('LCA', 'Excavation H ecosystem quality total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C108" t="inlineStr"/>
@@ -7614,7 +7614,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation H human health total CF [points/m3]')</t>
+          <t>('LCA', 'Excavation H human health total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C109" t="inlineStr"/>
@@ -7630,7 +7630,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>('LCA', 'Excavation H resources total CF [points/m3]')</t>
+          <t>('LCA', 'Gravel H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C110" t="inlineStr"/>
@@ -7646,7 +7646,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Gravel H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C111" t="inlineStr"/>
@@ -7662,7 +7662,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Gravel H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C112" t="inlineStr"/>
@@ -7678,7 +7678,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>('LCA', 'Gravel H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Plastic H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C113" t="inlineStr"/>
@@ -7694,7 +7694,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Plastic H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C114" t="inlineStr"/>
@@ -7710,7 +7710,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Plastic H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C115" t="inlineStr"/>
@@ -7726,7 +7726,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>('LCA', 'Plastic H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Sand H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C116" t="inlineStr"/>
@@ -7742,7 +7742,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Sand H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C117" t="inlineStr"/>
@@ -7758,7 +7758,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Sand H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C118" t="inlineStr"/>
@@ -7774,7 +7774,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>('LCA', 'Sand H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C119" t="inlineStr"/>
@@ -7790,7 +7790,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C120" t="inlineStr"/>
@@ -7806,7 +7806,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C121" t="inlineStr"/>
@@ -7822,7 +7822,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C122" t="inlineStr"/>
@@ -7838,7 +7838,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C123" t="inlineStr"/>
@@ -7854,7 +7854,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Stainless steel sheet H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C124" t="inlineStr"/>
@@ -7870,7 +7870,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>('LCA', 'Stainless steel sheet H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Steel H resources total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C125" t="inlineStr"/>
@@ -7886,7 +7886,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel H ecosystem quality total CF [points/kg]')</t>
+          <t>('LCA', 'Steel H ecosystem quality total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C126" t="inlineStr"/>
@@ -7902,7 +7902,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel H human health total CF [points/kg]')</t>
+          <t>('LCA', 'Steel H human health total CF [points/kilogram]')</t>
         </is>
       </c>
       <c r="C127" t="inlineStr"/>
@@ -7918,7 +7918,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>('LCA', 'Steel H resources total CF [points/kg]')</t>
+          <t>('LCA', 'Wood H resources total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C128" t="inlineStr"/>
@@ -7934,7 +7934,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood H ecosystem quality total CF [points/m3]')</t>
+          <t>('LCA', 'Wood H ecosystem quality total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C129" t="inlineStr"/>
@@ -7950,7 +7950,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood H human health total CF [points/m3]')</t>
+          <t>('LCA', 'Wood H human health total CF [points/cubic meter]')</t>
         </is>
       </c>
       <c r="C130" t="inlineStr"/>
@@ -7966,7 +7966,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>('LCA', 'Wood H resources total CF [points/m3]')</t>
+          <t>('LCA', 'Trucking H resources total CF [points/ton kilometer]')</t>
         </is>
       </c>
       <c r="C131" t="inlineStr"/>
@@ -7982,7 +7982,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking H ecosystem quality total CF [points/tonne*km]')</t>
+          <t>('LCA', 'Trucking H ecosystem quality total CF [points/ton kilometer]')</t>
         </is>
       </c>
       <c r="C132" t="inlineStr"/>
@@ -7998,7 +7998,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking H human health total CF [points/tonne*km]')</t>
+          <t>('LCA', 'Trucking H human health total CF [points/ton kilometer]')</t>
         </is>
       </c>
       <c r="C133" t="inlineStr"/>
@@ -8014,7 +8014,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>('LCA', 'Trucking H resources total CF [points/tonne*km]')</t>
+          <t>('LCA', 'N item H resources total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C134" t="inlineStr"/>
@@ -8062,7 +8062,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>('LCA', 'N item H resources total CF [points/kg]')</t>
+          <t>('LCA', 'P item H resources total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C137" t="inlineStr"/>
@@ -8110,7 +8110,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>('LCA', 'P item H resources total CF [points/kg]')</t>
+          <t>('LCA', 'K item H resources total CF [points/kg]')</t>
         </is>
       </c>
       <c r="C140" t="inlineStr"/>
@@ -8158,7 +8158,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>('LCA', 'K item H resources total CF [points/kg]')</t>
+          <t>('LCA', 'E item H resources total CF [points/kilowatt hour]')</t>
         </is>
       </c>
       <c r="C143" t="inlineStr"/>
@@ -8174,7 +8174,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>('LCA', 'E item H ecosystem quality total CF [points/kWh]')</t>
+          <t>('LCA', 'E item H ecosystem quality total CF [points/kilowatt hour]')</t>
         </is>
       </c>
       <c r="C144" t="inlineStr"/>
@@ -8190,7 +8190,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>('LCA', 'E item H human health total CF [points/kWh]')</t>
+          <t>('LCA', 'E item H human health total CF [points/kilowatt hour]')</t>
         </is>
       </c>
       <c r="C145" t="inlineStr"/>
@@ -8206,7 +8206,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>('LCA', 'E item H resources total CF [points/kWh]')</t>
+          <t>('TEA/LCA', 'Plant lifetime [yr]')</t>
         </is>
       </c>
       <c r="C146" t="inlineStr"/>

</xml_diff>